<commit_message>
action & organism test doing
</commit_message>
<xml_diff>
--- a/back/media/ㅂㅈㄷㅂㅈㄷㅂㄷ_모임참여자 정보.xlsx
+++ b/back/media/ㅂㅈㄷㅂㅈㄷㅂㄷ_모임참여자 정보.xlsx
@@ -374,7 +374,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,6 +440,31 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>홍길동</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>kdw1234</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>01085732136</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>kdw8573@snu.ac.kr</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>